<commit_message>
Added Code for Largest Rectangle In Histogram
</commit_message>
<xml_diff>
--- a/2.2. Stack/7. Largest Rectangle In Histogram/test_cases.xlsx
+++ b/2.2. Stack/7. Largest Rectangle In Histogram/test_cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Self-Study\LeetCode_Journey\2.2. Stack\7. Largest Rectangle In Histogram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3B28190-DE7A-4C83-9D22-A0381C5A2F5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60250713-7968-4A25-8E7E-505C88492D51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="3195" windowWidth="21600" windowHeight="11325" xr2:uid="{D3166FA0-5C9E-4470-8D2A-0706F74553A9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D3166FA0-5C9E-4470-8D2A-0706F74553A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>heights = [7,1,7,2,2,4]</t>
   </si>
@@ -48,6 +48,12 @@
   </si>
   <si>
     <t>output: 8</t>
+  </si>
+  <si>
+    <t>heights=[3,6,5,7,4,8,1,0]</t>
+  </si>
+  <si>
+    <t>output: 20</t>
   </si>
 </sst>
 </file>
@@ -77,7 +83,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -182,13 +188,60 @@
       <bottom style="thick">
         <color rgb="FFFF0000"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -200,6 +253,17 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -534,15 +598,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D28F4209-241E-48F4-9920-544C983CF79C}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="9" width="3.85546875" customWidth="1"/>
+    <col min="4" max="11" width="3.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -556,14 +620,17 @@
       </c>
       <c r="D2" s="1"/>
       <c r="F2" s="1"/>
+      <c r="I2" s="14"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D3" s="1"/>
       <c r="F3" s="1"/>
+      <c r="I3" s="14"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D4" s="1"/>
       <c r="F4" s="1"/>
+      <c r="I4" s="14"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D5" s="1"/>
@@ -590,7 +657,26 @@
       <c r="H8" s="9"/>
       <c r="I8" s="10"/>
     </row>
-    <row r="9" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="11">
+        <v>0</v>
+      </c>
+      <c r="E9" s="11">
+        <v>1</v>
+      </c>
+      <c r="F9" s="11">
+        <v>2</v>
+      </c>
+      <c r="G9" s="11">
+        <v>3</v>
+      </c>
+      <c r="H9" s="11">
+        <v>4</v>
+      </c>
+      <c r="I9" s="11">
+        <v>5</v>
+      </c>
+    </row>
     <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>1</v>
@@ -600,31 +686,145 @@
       <c r="A12" t="s">
         <v>2</v>
       </c>
+      <c r="D12" s="12"/>
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D13" s="12"/>
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D14" s="12"/>
       <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D15" s="12"/>
       <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D16" s="12"/>
       <c r="E16" s="1"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D17" s="12"/>
       <c r="E17" s="1"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D18" s="1"/>
+    <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D18" s="15"/>
       <c r="E18" s="1"/>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="4:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D19" s="11">
+        <v>0</v>
+      </c>
+      <c r="E19" s="11">
+        <v>1</v>
+      </c>
+      <c r="F19" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="12"/>
+      <c r="I22" s="1"/>
+      <c r="K22" s="14"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D23" s="12"/>
+      <c r="G23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="K23" s="14"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D24" s="12"/>
+      <c r="E24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="K24" s="14"/>
+    </row>
+    <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D25" s="12"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="16"/>
+      <c r="K25" s="14"/>
+    </row>
+    <row r="26" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D26" s="12"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="7"/>
+      <c r="K26" s="14"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D27" s="1"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="19"/>
+      <c r="K27" s="14"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D28" s="1"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="19"/>
+      <c r="K28" s="14"/>
+    </row>
+    <row r="29" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D29" s="1"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="17"/>
+    </row>
+    <row r="30" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D30" s="11">
+        <v>0</v>
+      </c>
+      <c r="E30" s="11">
+        <v>1</v>
+      </c>
+      <c r="F30" s="11">
+        <v>2</v>
+      </c>
+      <c r="G30" s="11">
+        <v>3</v>
+      </c>
+      <c r="H30" s="11">
+        <v>4</v>
+      </c>
+      <c r="I30" s="11">
+        <v>5</v>
+      </c>
+      <c r="J30" s="11">
+        <v>6</v>
+      </c>
+      <c r="K30" s="11">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>